<commit_message>
Se ajusta nomre en formato de planilla de firmas
</commit_message>
<xml_diff>
--- a/public/reportTemplates/Formato_firmas.xlsx
+++ b/public/reportTemplates/Formato_firmas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Laravel\CindaProd\BackendCinda\public\reportTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Universidad\Cinda\Codigo\BackendCinda\public\reportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B646261-8841-4B90-B824-22AF1E2A16B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CEF8EE-DCA7-4100-AE99-8F8192F1714C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="14374" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FORMATO FIRMAS CINDA 2020" sheetId="1" r:id="rId1"/>
@@ -310,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -374,29 +374,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -412,6 +397,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -419,7 +413,16 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,142 +687,142 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4:O5"/>
+      <selection activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" customWidth="1"/>
+    <col min="1" max="1" width="6.875" customWidth="1"/>
+    <col min="2" max="2" width="19.25" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.25" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="17.125" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="34" t="s">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
       <c r="G1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="26"/>
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="28"/>
       <c r="G2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="12.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="26"/>
+    <row r="3" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
       <c r="G3" s="11" t="s">
         <v>3</v>
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="15.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="26"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
       <c r="G4" s="11" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="O4" s="42"/>
-    </row>
-    <row r="5" spans="1:15" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="O4" s="23"/>
+    </row>
+    <row r="5" spans="1:15" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="26"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="26"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="2"/>
-      <c r="O5" s="42"/>
-    </row>
-    <row r="6" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="O5" s="23"/>
+    </row>
+    <row r="6" spans="1:15" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="38" t="s">
+      <c r="B6" s="33"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="38"/>
+      <c r="F6" s="33"/>
       <c r="G6" s="13"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:15" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+    <row r="7" spans="1:15" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="29"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="35"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="29"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="35"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:15" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
+    <row r="9" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="40"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="38"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:15" ht="26.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>14</v>
       </c>
@@ -829,507 +832,537 @@
       <c r="C10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
       <c r="G10" s="15" t="s">
         <v>18</v>
       </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
         <v>1</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
       <c r="G11" s="17"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16">
         <v>2</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
       <c r="G12" s="17"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="16">
         <v>3</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
       <c r="G13" s="17"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16">
         <v>4</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
       <c r="G14" s="17"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16">
         <v>5</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
       <c r="G15" s="17"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="16">
         <v>6</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
       <c r="G16" s="17"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="16">
         <v>7</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
       <c r="G17" s="17"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="16">
         <v>8</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
       <c r="G18" s="17"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="16">
         <v>9</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
       <c r="G19" s="17"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="16">
         <v>10</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
       <c r="G20" s="17"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="16">
         <v>11</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
       <c r="G21" s="17"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="16">
         <v>12</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
       <c r="G22" s="17"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="16">
         <v>13</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
       <c r="G23" s="17"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="16">
         <v>14</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
       <c r="G24" s="17"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="16">
         <v>15</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
       <c r="G25" s="17"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="16">
         <v>16</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
       <c r="G26" s="17"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="16">
         <v>17</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
       <c r="G27" s="17"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="16">
         <v>18</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
       <c r="G28" s="17"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="16">
         <v>19</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="9"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
       <c r="G29" s="17"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="16">
         <v>20</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="9"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
       <c r="G30" s="17"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="16">
         <v>21</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="9"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="17"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="16">
         <v>22</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="9"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
       <c r="G32" s="17"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="16">
         <v>23</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="9"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
       <c r="G33" s="17"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="16">
         <v>24</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="9"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
       <c r="G34" s="17"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="16">
         <v>25</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="9"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
       <c r="G35" s="17"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="16">
         <v>26</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="9"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
       <c r="G36" s="17"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="16">
         <v>27</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="9"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
       <c r="G37" s="17"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="16">
         <v>28</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="9"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
       <c r="G38" s="17"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="16">
         <v>29</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="9"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
       <c r="G39" s="17"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="16">
         <v>30</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="9"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
       <c r="G40" s="17"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="16">
         <v>31</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="9"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
       <c r="G41" s="17"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="16">
         <v>32</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="9"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
       <c r="G42" s="17"/>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="16">
         <v>33</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="9"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
       <c r="G43" s="17"/>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="16">
         <v>34</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="9"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
       <c r="G44" s="17"/>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="16">
         <v>35</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="9"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
       <c r="G45" s="17"/>
       <c r="H45" s="1"/>
       <c r="I45" s="22"/>
       <c r="J45" s="22"/>
     </row>
-    <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="16">
         <v>36</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="9"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
       <c r="G46" s="17"/>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="16">
         <v>37</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="9"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
       <c r="G47" s="17"/>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="16">
         <v>38</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="9"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28"/>
       <c r="G48" s="17"/>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="16">
         <v>39</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="9"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
       <c r="G49" s="17"/>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="18">
         <v>40</v>
       </c>
       <c r="B50" s="19"/>
       <c r="C50" s="20"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
       <c r="G50" s="21"/>
       <c r="H50" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="A1:C4"/>
-    <mergeCell ref="D1:F4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D17:F17"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="D11:F11"/>
@@ -1340,43 +1373,13 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="A1:C4"/>
+    <mergeCell ref="D1:F4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="1.347068145800317E-2" top="0.76782884310618071" bottom="0.49841521394611726" header="0" footer="0"/>

</xml_diff>